<commit_message>
+ Make Character Stat and Character Scene UI.
</commit_message>
<xml_diff>
--- a/Assets/Data/Localizations.xlsx
+++ b/Assets/Data/Localizations.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="599">
   <si>
     <t>ID</t>
   </si>
@@ -2238,9 +2238,6 @@
     <t>STR_CRIT</t>
   </si>
   <si>
-    <t>Critical Chance</t>
-  </si>
-  <si>
     <t>Tỉ lệ Bạo Kích</t>
   </si>
   <si>
@@ -2256,30 +2253,15 @@
     <t>STR_SPD</t>
   </si>
   <si>
-    <t>S</t>
-  </si>
-  <si>
     <t>Speed</t>
   </si>
   <si>
     <t>Tốc độ</t>
   </si>
   <si>
-    <t>STR_ARM_PEN</t>
-  </si>
-  <si>
-    <t>Armor Penetration</t>
-  </si>
-  <si>
     <t>Khả năng xuyên giáp</t>
   </si>
   <si>
-    <t>STR_ACC</t>
-  </si>
-  <si>
-    <t>Effect Accuracy</t>
-  </si>
-  <si>
     <t>Hiệu ứng chính xác</t>
   </si>
   <si>
@@ -2443,6 +2425,375 @@
   </si>
   <si>
     <t>STR_ARMOR_SET_DES</t>
+  </si>
+  <si>
+    <t>STR_SUN_WUKONG</t>
+  </si>
+  <si>
+    <t>STR_TANG_SANZANG</t>
+  </si>
+  <si>
+    <t>STR_ZHU_BAIJE</t>
+  </si>
+  <si>
+    <t>STR_SHA_WUJING</t>
+  </si>
+  <si>
+    <t>Sun Wukong</t>
+  </si>
+  <si>
+    <t>Tang Sanzang</t>
+  </si>
+  <si>
+    <t>Sha Wujing</t>
+  </si>
+  <si>
+    <t>Zhu Bajie</t>
+  </si>
+  <si>
+    <t>Tôn Ngộ Không</t>
+  </si>
+  <si>
+    <t>Đường Tăng</t>
+  </si>
+  <si>
+    <t>Trư Bát Giới</t>
+  </si>
+  <si>
+    <t>Sa Tăng</t>
+  </si>
+  <si>
+    <t>STR_SHARD_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>Vật liệu cần thiết để đột phá {0} . Thu thập đủ {1} Tinh Phách có thể ghép thành {0}.</t>
+  </si>
+  <si>
+    <t>The primary material needed to help {0} Ascension. Collect {1} to fuse for {0}.</t>
+  </si>
+  <si>
+    <t>STR_SHARD_NAME</t>
+  </si>
+  <si>
+    <t>Esence</t>
+  </si>
+  <si>
+    <t>Tinh Phách</t>
+  </si>
+  <si>
+    <t>STR_DRAGON_KING_EATERN_SEA</t>
+  </si>
+  <si>
+    <t>Dragon King of the Eastern Sea</t>
+  </si>
+  <si>
+    <t>Đông Hải Long Vương</t>
+  </si>
+  <si>
+    <t>STR_THIRD_PRINCE_NEZHA</t>
+  </si>
+  <si>
+    <t>Third Prince Nezha</t>
+  </si>
+  <si>
+    <t>Tam Thái Tử Na Tra</t>
+  </si>
+  <si>
+    <t>Bull Demon King</t>
+  </si>
+  <si>
+    <t>Ngưu Ma Vương</t>
+  </si>
+  <si>
+    <t>STR_BULL_DEMON_KING</t>
+  </si>
+  <si>
+    <t>STR_ERLANG_SHEN_YANG_JIAN</t>
+  </si>
+  <si>
+    <t>Erlang Shen Yang Jian</t>
+  </si>
+  <si>
+    <t>Nhị Lang Thần Dương Tiễn</t>
+  </si>
+  <si>
+    <t>STR_LITTLE_WHITE_DRAGON</t>
+  </si>
+  <si>
+    <t>Little White Dragon</t>
+  </si>
+  <si>
+    <t>Tiểu Bạch Long</t>
+  </si>
+  <si>
+    <t>STR_GUANYIN_BODHISATTVA</t>
+  </si>
+  <si>
+    <t>Guanyin Bodhisattva</t>
+  </si>
+  <si>
+    <t>Quan Thế Âm Bồ Tát</t>
+  </si>
+  <si>
+    <t>UI_ASCEND</t>
+  </si>
+  <si>
+    <t>Ascend</t>
+  </si>
+  <si>
+    <t>Đột phá</t>
+  </si>
+  <si>
+    <t>UI_CULTIVATE</t>
+  </si>
+  <si>
+    <t>Cultivate</t>
+  </si>
+  <si>
+    <t>Tu luyện</t>
+  </si>
+  <si>
+    <t>Effect Hit</t>
+  </si>
+  <si>
+    <t>Defense Shred</t>
+  </si>
+  <si>
+    <t>Critical Rate</t>
+  </si>
+  <si>
+    <t>STR_DEF_SHRED</t>
+  </si>
+  <si>
+    <t>STR_EFF_HIT</t>
+  </si>
+  <si>
+    <t>STR_EFF_RES</t>
+  </si>
+  <si>
+    <t>Effect Resistance</t>
+  </si>
+  <si>
+    <t>Kháng hiệu ứng</t>
+  </si>
+  <si>
+    <t>UI_COST</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>UI_ADVANCEMENT</t>
+  </si>
+  <si>
+    <t>Advancement</t>
+  </si>
+  <si>
+    <t>Thăng cấp</t>
+  </si>
+  <si>
+    <t>UI_ATK</t>
+  </si>
+  <si>
+    <t>ATK</t>
+  </si>
+  <si>
+    <t>UI_DEF</t>
+  </si>
+  <si>
+    <t>DEF</t>
+  </si>
+  <si>
+    <t>UI_SPD</t>
+  </si>
+  <si>
+    <t>SPD</t>
+  </si>
+  <si>
+    <t>UI_ASSITS_RATE</t>
+  </si>
+  <si>
+    <t>Assist Rate</t>
+  </si>
+  <si>
+    <t>UI_CRIT_RATE</t>
+  </si>
+  <si>
+    <t>CRIT Rate</t>
+  </si>
+  <si>
+    <t>UI_CRIT_DMG</t>
+  </si>
+  <si>
+    <t>CRIT DMG</t>
+  </si>
+  <si>
+    <t>UI_EFFECT_HIT</t>
+  </si>
+  <si>
+    <t>UI_EFFECT_RES</t>
+  </si>
+  <si>
+    <t>Feffect Res</t>
+  </si>
+  <si>
+    <t>UI_QUICK_UNEQUIP</t>
+  </si>
+  <si>
+    <t>UI_QUICK_EQUIP</t>
+  </si>
+  <si>
+    <t>Quick UnEquip</t>
+  </si>
+  <si>
+    <t>Quick Equip</t>
+  </si>
+  <si>
+    <t>UI_CHANGE</t>
+  </si>
+  <si>
+    <t>Change</t>
+  </si>
+  <si>
+    <t>UI_ENHANCE</t>
+  </si>
+  <si>
+    <t>Enhance</t>
+  </si>
+  <si>
+    <t>Cường Hóa</t>
+  </si>
+  <si>
+    <t>Đổi</t>
+  </si>
+  <si>
+    <t>Mặc nhanh</t>
+  </si>
+  <si>
+    <t>Gỡ nhanh</t>
+  </si>
+  <si>
+    <t>ST Bạo kích</t>
+  </si>
+  <si>
+    <t>Tỉ lệ bạo kích</t>
+  </si>
+  <si>
+    <t>Tỉ lệ hỗ trợ</t>
+  </si>
+  <si>
+    <t>UI_BATTLE_POWER</t>
+  </si>
+  <si>
+    <t>Battle Power</t>
+  </si>
+  <si>
+    <t>Chiến Lực</t>
+  </si>
+  <si>
+    <t>UI_FATE</t>
+  </si>
+  <si>
+    <t>Fate</t>
+  </si>
+  <si>
+    <t>Bản Mệnh</t>
+  </si>
+  <si>
+    <t>UI_TUTORIAL</t>
+  </si>
+  <si>
+    <t>Tutorial</t>
+  </si>
+  <si>
+    <t>Hướng dẫn</t>
+  </si>
+  <si>
+    <t>STR_CRIT_RATE</t>
+  </si>
+  <si>
+    <t>Crittle Rate</t>
+  </si>
+  <si>
+    <t>STR_COMMON_EXP</t>
+  </si>
+  <si>
+    <t>STR_FINE_EXP</t>
+  </si>
+  <si>
+    <t>STR_RARE_EXP</t>
+  </si>
+  <si>
+    <t>STR_SUPREME_EXP</t>
+  </si>
+  <si>
+    <t>Common EXP Pill</t>
+  </si>
+  <si>
+    <t>Fine EXP Pill</t>
+  </si>
+  <si>
+    <t>Rare EXP Gourd</t>
+  </si>
+  <si>
+    <t>Supreme EXP Gourd</t>
+  </si>
+  <si>
+    <t>STR_EXP_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>Can be used in Character Cultivate to increase Character EXP by {0}.</t>
+  </si>
+  <si>
+    <t>STR_EXP_USEFUL</t>
+  </si>
+  <si>
+    <t>An immortal elixir forged by the Grand Supreme Elder Lord within the Eight Trigrams Furnace. It absorbs the essence of heaven and earth, granting eternal life and advancing in cultivation.</t>
+  </si>
+  <si>
+    <t>Dùng trong Tu Luyện Nhân Vật, tăng {0} điểm EXP nhân vật.</t>
+  </si>
+  <si>
+    <t>Thuốc EXP hạ phẩm</t>
+  </si>
+  <si>
+    <t>Thuốc EXP trung phẩm</t>
+  </si>
+  <si>
+    <t>Bình EXP thượng phẩm</t>
+  </si>
+  <si>
+    <t>Bình EXP tuyệt phẩm</t>
+  </si>
+  <si>
+    <t>Một loại tiên dược do Thái Thượng Lão Quân luyện thành trong lò Bát Quái, hấp thu tinh hoa của trời đất, ban cho trường sinh bất lão, tăng tiến tu vi.</t>
+  </si>
+  <si>
+    <t>UI_PENETRATION</t>
+  </si>
+  <si>
+    <t>Pennetration</t>
+  </si>
+  <si>
+    <t>Xuyên giáp</t>
+  </si>
+  <si>
+    <t>UI_CRITDMG_RES</t>
+  </si>
+  <si>
+    <t>Crit DMG Res</t>
+  </si>
+  <si>
+    <t>Kháng ST bạo kích</t>
+  </si>
+  <si>
+    <t>STR_MAX_LEVEL</t>
+  </si>
+  <si>
+    <t>Max level</t>
+  </si>
+  <si>
+    <t>Cấp độ tối đa</t>
   </si>
 </sst>
 </file>
@@ -2787,10 +3138,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView topLeftCell="A30" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3161,6 +3512,248 @@
       </c>
       <c r="C33" t="s">
         <v>297</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>512</v>
+      </c>
+      <c r="B34" t="s">
+        <v>513</v>
+      </c>
+      <c r="C34" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>515</v>
+      </c>
+      <c r="B35" t="s">
+        <v>516</v>
+      </c>
+      <c r="C35" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>526</v>
+      </c>
+      <c r="B36" t="s">
+        <v>527</v>
+      </c>
+      <c r="C36" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>528</v>
+      </c>
+      <c r="B37" t="s">
+        <v>529</v>
+      </c>
+      <c r="C37" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>210</v>
+      </c>
+      <c r="B38" t="s">
+        <v>211</v>
+      </c>
+      <c r="C38" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>531</v>
+      </c>
+      <c r="B39" t="s">
+        <v>532</v>
+      </c>
+      <c r="C39" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>533</v>
+      </c>
+      <c r="B40" t="s">
+        <v>534</v>
+      </c>
+      <c r="C40" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>535</v>
+      </c>
+      <c r="B41" t="s">
+        <v>536</v>
+      </c>
+      <c r="C41" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>537</v>
+      </c>
+      <c r="B42" t="s">
+        <v>538</v>
+      </c>
+      <c r="C42" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>539</v>
+      </c>
+      <c r="B43" t="s">
+        <v>540</v>
+      </c>
+      <c r="C43" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>541</v>
+      </c>
+      <c r="B44" t="s">
+        <v>542</v>
+      </c>
+      <c r="C44" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>543</v>
+      </c>
+      <c r="B45" t="s">
+        <v>518</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>544</v>
+      </c>
+      <c r="B46" t="s">
+        <v>545</v>
+      </c>
+      <c r="C46" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>546</v>
+      </c>
+      <c r="B47" t="s">
+        <v>548</v>
+      </c>
+      <c r="C47" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>547</v>
+      </c>
+      <c r="B48" t="s">
+        <v>549</v>
+      </c>
+      <c r="C48" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>550</v>
+      </c>
+      <c r="B49" t="s">
+        <v>551</v>
+      </c>
+      <c r="C49" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>552</v>
+      </c>
+      <c r="B50" t="s">
+        <v>553</v>
+      </c>
+      <c r="C50" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>561</v>
+      </c>
+      <c r="B51" t="s">
+        <v>562</v>
+      </c>
+      <c r="C51" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>564</v>
+      </c>
+      <c r="B52" t="s">
+        <v>565</v>
+      </c>
+      <c r="C52" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>567</v>
+      </c>
+      <c r="B53" t="s">
+        <v>568</v>
+      </c>
+      <c r="C53" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>590</v>
+      </c>
+      <c r="B54" t="s">
+        <v>591</v>
+      </c>
+      <c r="C54" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>593</v>
+      </c>
+      <c r="B55" t="s">
+        <v>594</v>
+      </c>
+      <c r="C55" t="s">
+        <v>595</v>
       </c>
     </row>
   </sheetData>
@@ -3223,10 +3816,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C128"/>
+  <dimension ref="A1:C149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A105" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A127" sqref="A127"/>
+    <sheetView tabSelected="1" topLeftCell="A138" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C152" sqref="C152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3241,7 +3834,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>419</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -4396,252 +4989,483 @@
         <v>412</v>
       </c>
       <c r="B106" s="3" t="s">
+        <v>520</v>
+      </c>
+      <c r="C106" s="3" t="s">
         <v>413</v>
-      </c>
-      <c r="C106" s="3" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
+        <v>414</v>
+      </c>
+      <c r="B107" s="3" t="s">
         <v>415</v>
       </c>
-      <c r="B107" s="3" t="s">
+      <c r="C107" s="3" t="s">
         <v>416</v>
-      </c>
-      <c r="C107" s="3" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
+        <v>417</v>
+      </c>
+      <c r="B108" s="3" t="s">
         <v>418</v>
       </c>
-      <c r="B108" s="3" t="s">
-        <v>420</v>
-      </c>
       <c r="C108" s="3" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>422</v>
+        <v>521</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>423</v>
+        <v>519</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>425</v>
+        <v>522</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>426</v>
+        <v>518</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>427</v>
+        <v>421</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>435</v>
+        <v>523</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>434</v>
+        <v>524</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>433</v>
+        <v>525</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>436</v>
+        <v>429</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>437</v>
+        <v>430</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>431</v>
+        <v>423</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>430</v>
+        <v>422</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>439</v>
+        <v>431</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>442</v>
-      </c>
-      <c r="C114" t="s">
-        <v>441</v>
+        <v>425</v>
+      </c>
+      <c r="C114" s="3" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>443</v>
-      </c>
-      <c r="C115" s="3" t="s">
-        <v>432</v>
+        <v>436</v>
+      </c>
+      <c r="C115" t="s">
+        <v>435</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>440</v>
+        <v>432</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>445</v>
+        <v>437</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>444</v>
+        <v>426</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>446</v>
+        <v>434</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>447</v>
+        <v>439</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>448</v>
+        <v>438</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>449</v>
+        <v>440</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>450</v>
+        <v>441</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>451</v>
+        <v>442</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>452</v>
+        <v>443</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>453</v>
+        <v>444</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>454</v>
+        <v>445</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>455</v>
+        <v>446</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>456</v>
+        <v>447</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>457</v>
+        <v>448</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>458</v>
+        <v>449</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>459</v>
+        <v>450</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>460</v>
+        <v>451</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>461</v>
+        <v>452</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>462</v>
+        <v>453</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>463</v>
+        <v>454</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>474</v>
+        <v>455</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>464</v>
+        <v>456</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>469</v>
+        <v>457</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>476</v>
+        <v>468</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>471</v>
+        <v>463</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>477</v>
+        <v>470</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>472</v>
+        <v>464</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>478</v>
+        <v>469</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="C127" s="3" t="s">
-        <v>473</v>
+        <v>466</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
+        <v>472</v>
+      </c>
+      <c r="B128" s="3" t="s">
+        <v>462</v>
+      </c>
+      <c r="C128" s="3" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>475</v>
+      </c>
+      <c r="B129" s="3" t="s">
+        <v>473</v>
+      </c>
+      <c r="C129" s="3" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>476</v>
+      </c>
+      <c r="B130" s="3" t="s">
+        <v>480</v>
+      </c>
+      <c r="C130" s="3" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>477</v>
+      </c>
+      <c r="B131" s="3" t="s">
         <v>481</v>
       </c>
-      <c r="B128" s="3" t="s">
+      <c r="C131" s="3" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>478</v>
+      </c>
+      <c r="B132" s="3" t="s">
+        <v>483</v>
+      </c>
+      <c r="C132" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
         <v>479</v>
       </c>
-      <c r="C128" s="3" t="s">
-        <v>480</v>
+      <c r="B133" s="3" t="s">
+        <v>482</v>
+      </c>
+      <c r="C133" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>488</v>
+      </c>
+      <c r="B134" s="3" t="s">
+        <v>490</v>
+      </c>
+      <c r="C134" s="3" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>491</v>
+      </c>
+      <c r="B135" s="3" t="s">
+        <v>492</v>
+      </c>
+      <c r="C135" s="3" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>494</v>
+      </c>
+      <c r="B136" s="3" t="s">
+        <v>495</v>
+      </c>
+      <c r="C136" s="3" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>497</v>
+      </c>
+      <c r="B137" t="s">
+        <v>498</v>
+      </c>
+      <c r="C137" s="3" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>502</v>
+      </c>
+      <c r="B138" t="s">
+        <v>500</v>
+      </c>
+      <c r="C138" s="3" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>503</v>
+      </c>
+      <c r="B139" s="3" t="s">
+        <v>504</v>
+      </c>
+      <c r="C139" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>506</v>
+      </c>
+      <c r="B140" t="s">
+        <v>507</v>
+      </c>
+      <c r="C140" s="3" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>509</v>
+      </c>
+      <c r="B141" t="s">
+        <v>510</v>
+      </c>
+      <c r="C141" s="3" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>570</v>
+      </c>
+      <c r="B142" t="s">
+        <v>571</v>
+      </c>
+      <c r="C142" s="3" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>572</v>
+      </c>
+      <c r="B143" t="s">
+        <v>576</v>
+      </c>
+      <c r="C143" s="3" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>573</v>
+      </c>
+      <c r="B144" t="s">
+        <v>577</v>
+      </c>
+      <c r="C144" s="3" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>574</v>
+      </c>
+      <c r="B145" t="s">
+        <v>578</v>
+      </c>
+      <c r="C145" s="3" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>575</v>
+      </c>
+      <c r="B146" t="s">
+        <v>579</v>
+      </c>
+      <c r="C146" s="3" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>582</v>
+      </c>
+      <c r="B147" t="s">
+        <v>581</v>
+      </c>
+      <c r="C147" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>580</v>
+      </c>
+      <c r="B148" t="s">
+        <v>583</v>
+      </c>
+      <c r="C148" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>596</v>
+      </c>
+      <c r="B149" t="s">
+        <v>597</v>
+      </c>
+      <c r="C149" s="3" t="s">
+        <v>598</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
+ Add Armor Category UI in Character Scene.
</commit_message>
<xml_diff>
--- a/Assets/Data/Localizations.xlsx
+++ b/Assets/Data/Localizations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="UI" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="618">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="621">
   <si>
     <t>ID</t>
   </si>
@@ -2851,6 +2851,15 @@
   </si>
   <si>
     <t>Enchance</t>
+  </si>
+  <si>
+    <t>UI_EQUIP</t>
+  </si>
+  <si>
+    <t>Equip</t>
+  </si>
+  <si>
+    <t>Mặc</t>
   </si>
 </sst>
 </file>
@@ -3195,10 +3204,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C62"/>
+  <dimension ref="A1:C63"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3888,6 +3897,17 @@
       </c>
       <c r="C62" t="s">
         <v>600</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>618</v>
+      </c>
+      <c r="B63" t="s">
+        <v>619</v>
+      </c>
+      <c r="C63" t="s">
+        <v>620</v>
       </c>
     </row>
   </sheetData>
@@ -3952,7 +3972,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A125" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A125" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="A149" sqref="A149"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
+ Create Animation for Protagonist and remove _IOjbectInject.Inject(this)
</commit_message>
<xml_diff>
--- a/Assets/Data/Localizations.xlsx
+++ b/Assets/Data/Localizations.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="670">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="671">
   <si>
     <t>ID</t>
   </si>
@@ -3007,6 +3007,9 @@
   </si>
   <si>
     <t>Dùng để cường hóa pháp bảo.</t>
+  </si>
+  <si>
+    <t>STR_LANGUAGE</t>
   </si>
 </sst>
 </file>
@@ -4149,10 +4152,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C165"/>
+  <dimension ref="A1:C166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A144" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B157" sqref="B157"/>
+    <sheetView tabSelected="1" topLeftCell="A156" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C177" sqref="C177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5974,6 +5977,17 @@
         <v>668</v>
       </c>
     </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>670</v>
+      </c>
+      <c r="B166" t="s">
+        <v>22</v>
+      </c>
+      <c r="C166" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
+ Add game config for game narrative.
</commit_message>
<xml_diff>
--- a/Assets/Data/Localizations.xlsx
+++ b/Assets/Data/Localizations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="UI" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="671">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="683">
   <si>
     <t>ID</t>
   </si>
@@ -113,24 +113,6 @@
     <t>Thông tin</t>
   </si>
   <si>
-    <t>CHAP01_NPC01_01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Greetings, Great Sage </t>
-  </si>
-  <si>
-    <t>My gratitude, venerable one!</t>
-  </si>
-  <si>
-    <t>CHAP01_NPC01_02</t>
-  </si>
-  <si>
-    <t>Xin chào đại thánh.</t>
-  </si>
-  <si>
-    <t>Cảm ơn ngài!</t>
-  </si>
-  <si>
     <t>Tiếng Việt</t>
   </si>
   <si>
@@ -2454,15 +2436,9 @@
     <t>Tôn Ngộ Không</t>
   </si>
   <si>
-    <t>Đường Tăng</t>
-  </si>
-  <si>
     <t>Trư Bát Giới</t>
   </si>
   <si>
-    <t>Sa Tăng</t>
-  </si>
-  <si>
     <t>STR_SHARD_DESCRIPTION</t>
   </si>
   <si>
@@ -3010,6 +2986,66 @@
   </si>
   <si>
     <t>STR_LANGUAGE</t>
+  </si>
+  <si>
+    <t>STR_JADE_EMPEROR</t>
+  </si>
+  <si>
+    <t>Jade Emperor</t>
+  </si>
+  <si>
+    <t>Ngọc Hoàng</t>
+  </si>
+  <si>
+    <t>STR_BODHI_PATRIARCH</t>
+  </si>
+  <si>
+    <t>Bodhi Patriarch</t>
+  </si>
+  <si>
+    <t>STR_TAIBAI_JINXING</t>
+  </si>
+  <si>
+    <t>Taibai Jinxing</t>
+  </si>
+  <si>
+    <t>Bồ Đề Tổ Sư</t>
+  </si>
+  <si>
+    <t>Thái Bạch Kim Tinh</t>
+  </si>
+  <si>
+    <t>Taishang Laojun</t>
+  </si>
+  <si>
+    <t>STR_TAISHANG_LAOJUN</t>
+  </si>
+  <si>
+    <t>Thái Thượng Lão Quân</t>
+  </si>
+  <si>
+    <t>Sa Ngộ Tĩnh</t>
+  </si>
+  <si>
+    <t>Đường Tăng Tạ</t>
+  </si>
+  <si>
+    <t>Phật Tổ Như Lai</t>
+  </si>
+  <si>
+    <t>Tathāgata Buddha</t>
+  </si>
+  <si>
+    <t>STR_SHAKYAMUNI_BUDDHA</t>
+  </si>
+  <si>
+    <t>STR_YANLUA_WANG</t>
+  </si>
+  <si>
+    <t>Yama, the King of Hell</t>
+  </si>
+  <si>
+    <t>Giêm La Vương</t>
   </si>
 </sst>
 </file>
@@ -3479,617 +3515,617 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C13" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C14" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B15" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C15" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B16" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C16" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B17" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C17" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B18" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C18" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B19" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C19" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B20" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C20" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B21" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C21" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B22" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C22" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B23" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C23" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B24" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C24" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B25" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C25" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="B26" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="C26" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="B27" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="C27" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="B28" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="C28" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="B29" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="C29" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="B30" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="C30" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="B31" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="C31" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="B32" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="C32" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="B33" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="C33" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>512</v>
+        <v>504</v>
       </c>
       <c r="B34" t="s">
-        <v>513</v>
+        <v>505</v>
       </c>
       <c r="C34" t="s">
-        <v>514</v>
+        <v>506</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>515</v>
+        <v>507</v>
       </c>
       <c r="B35" t="s">
-        <v>516</v>
+        <v>508</v>
       </c>
       <c r="C35" t="s">
-        <v>517</v>
+        <v>509</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>526</v>
+        <v>518</v>
       </c>
       <c r="B36" t="s">
-        <v>527</v>
+        <v>519</v>
       </c>
       <c r="C36" t="s">
-        <v>615</v>
+        <v>607</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>528</v>
+        <v>520</v>
       </c>
       <c r="B37" t="s">
-        <v>529</v>
+        <v>521</v>
       </c>
       <c r="C37" t="s">
-        <v>530</v>
+        <v>522</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="B38" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="C38" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>531</v>
+        <v>523</v>
       </c>
       <c r="B39" t="s">
-        <v>532</v>
+        <v>524</v>
       </c>
       <c r="C39" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>533</v>
+        <v>525</v>
       </c>
       <c r="B40" t="s">
-        <v>534</v>
+        <v>526</v>
       </c>
       <c r="C40" t="s">
-        <v>408</v>
+        <v>402</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>535</v>
+        <v>527</v>
       </c>
       <c r="B41" t="s">
-        <v>536</v>
+        <v>528</v>
       </c>
       <c r="C41" t="s">
-        <v>419</v>
+        <v>413</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>537</v>
+        <v>529</v>
       </c>
       <c r="B42" t="s">
-        <v>538</v>
+        <v>530</v>
       </c>
       <c r="C42" t="s">
-        <v>560</v>
+        <v>552</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>539</v>
+        <v>531</v>
       </c>
       <c r="B43" t="s">
-        <v>540</v>
+        <v>532</v>
       </c>
       <c r="C43" t="s">
-        <v>559</v>
+        <v>551</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>541</v>
+        <v>533</v>
       </c>
       <c r="B44" t="s">
-        <v>542</v>
+        <v>534</v>
       </c>
       <c r="C44" t="s">
-        <v>558</v>
+        <v>550</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>543</v>
+        <v>535</v>
       </c>
       <c r="B45" t="s">
-        <v>518</v>
+        <v>510</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>421</v>
+        <v>415</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>544</v>
+        <v>536</v>
       </c>
       <c r="B46" t="s">
-        <v>545</v>
+        <v>537</v>
       </c>
       <c r="C46" t="s">
-        <v>525</v>
+        <v>517</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>546</v>
+        <v>538</v>
       </c>
       <c r="B47" t="s">
-        <v>548</v>
+        <v>540</v>
       </c>
       <c r="C47" t="s">
-        <v>557</v>
+        <v>549</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>547</v>
+        <v>539</v>
       </c>
       <c r="B48" t="s">
-        <v>549</v>
+        <v>541</v>
       </c>
       <c r="C48" t="s">
-        <v>556</v>
+        <v>548</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>550</v>
+        <v>542</v>
       </c>
       <c r="B49" t="s">
-        <v>551</v>
+        <v>543</v>
       </c>
       <c r="C49" t="s">
-        <v>555</v>
+        <v>547</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>552</v>
+        <v>544</v>
       </c>
       <c r="B50" t="s">
-        <v>553</v>
+        <v>545</v>
       </c>
       <c r="C50" t="s">
-        <v>554</v>
+        <v>546</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>561</v>
+        <v>553</v>
       </c>
       <c r="B51" t="s">
-        <v>562</v>
+        <v>554</v>
       </c>
       <c r="C51" t="s">
-        <v>563</v>
+        <v>555</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>564</v>
+        <v>556</v>
       </c>
       <c r="B52" t="s">
-        <v>565</v>
+        <v>557</v>
       </c>
       <c r="C52" t="s">
-        <v>566</v>
+        <v>558</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>567</v>
+        <v>559</v>
       </c>
       <c r="B53" t="s">
-        <v>568</v>
+        <v>560</v>
       </c>
       <c r="C53" t="s">
-        <v>569</v>
+        <v>561</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>590</v>
+        <v>582</v>
       </c>
       <c r="B54" t="s">
-        <v>591</v>
+        <v>583</v>
       </c>
       <c r="C54" t="s">
-        <v>592</v>
+        <v>584</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>593</v>
+        <v>585</v>
       </c>
       <c r="B55" t="s">
-        <v>594</v>
+        <v>586</v>
       </c>
       <c r="C55" t="s">
-        <v>595</v>
+        <v>587</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>599</v>
+        <v>591</v>
       </c>
       <c r="B56" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="C56" t="s">
-        <v>600</v>
+        <v>592</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>601</v>
+        <v>593</v>
       </c>
       <c r="B57" t="s">
-        <v>602</v>
+        <v>594</v>
       </c>
       <c r="C57" t="s">
-        <v>603</v>
+        <v>595</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>604</v>
+        <v>596</v>
       </c>
       <c r="B58" t="s">
-        <v>605</v>
+        <v>597</v>
       </c>
       <c r="C58" t="s">
-        <v>606</v>
+        <v>598</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>607</v>
+        <v>599</v>
       </c>
       <c r="B59" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="C59" t="s">
-        <v>608</v>
+        <v>600</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>609</v>
+        <v>601</v>
       </c>
       <c r="B60" t="s">
-        <v>610</v>
+        <v>602</v>
       </c>
       <c r="C60" t="s">
-        <v>611</v>
+        <v>603</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>614</v>
+        <v>606</v>
       </c>
       <c r="B61" t="s">
-        <v>613</v>
+        <v>605</v>
       </c>
       <c r="C61" t="s">
-        <v>612</v>
+        <v>604</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>616</v>
+        <v>608</v>
       </c>
       <c r="B62" t="s">
-        <v>617</v>
+        <v>609</v>
       </c>
       <c r="C62" t="s">
-        <v>600</v>
+        <v>592</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>618</v>
+        <v>610</v>
       </c>
       <c r="B63" t="s">
-        <v>619</v>
+        <v>611</v>
       </c>
       <c r="C63" t="s">
-        <v>620</v>
+        <v>612</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>651</v>
+        <v>643</v>
       </c>
       <c r="B64" t="s">
-        <v>652</v>
+        <v>644</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>653</v>
+        <v>645</v>
       </c>
       <c r="B65" t="s">
-        <v>656</v>
+        <v>648</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>654</v>
+        <v>646</v>
       </c>
       <c r="B66" t="s">
-        <v>655</v>
+        <v>647</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>657</v>
+        <v>649</v>
       </c>
       <c r="B67" t="s">
-        <v>658</v>
+        <v>650</v>
       </c>
     </row>
   </sheetData>
@@ -4099,15 +4135,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23" customWidth="1"/>
+    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.7109375" customWidth="1"/>
     <col min="3" max="3" width="47.140625" customWidth="1"/>
   </cols>
@@ -4125,24 +4161,68 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>663</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>664</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>665</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>666</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>667</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>670</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>668</v>
+      </c>
+      <c r="B4" t="s">
+        <v>669</v>
+      </c>
+      <c r="C4" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>673</v>
+      </c>
+      <c r="B5" t="s">
+        <v>672</v>
+      </c>
+      <c r="C5" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>679</v>
+      </c>
+      <c r="B6" t="s">
+        <v>678</v>
+      </c>
+      <c r="C6" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>680</v>
+      </c>
+      <c r="B7" t="s">
+        <v>681</v>
+      </c>
+      <c r="C7" t="s">
+        <v>682</v>
       </c>
     </row>
   </sheetData>
@@ -4154,8 +4234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A156" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C177" sqref="C177"/>
+    <sheetView topLeftCell="A125" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A137" sqref="A137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4178,1808 +4258,1808 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B4" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C4" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B5" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C5" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B6" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C6" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B7" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C7" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B8" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C8" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B9" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C9" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B10" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C10" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="B11" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="C11" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B12" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="C12" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>120</v>
+      </c>
+      <c r="B13" t="s">
+        <v>121</v>
+      </c>
+      <c r="C13" t="s">
         <v>126</v>
-      </c>
-      <c r="B13" t="s">
-        <v>127</v>
-      </c>
-      <c r="C13" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B14" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="C14" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B15" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="C15" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B16" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="C16" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B17" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C17" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B18" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="C18" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B19" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C19" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B20" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="C20" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B21" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="C21" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B22" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C22" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B23" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="C23" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B24" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="C24" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B25" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C25" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B26" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C26" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B27" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="C27" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="B28" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="C28" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="B29" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="C29" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B30" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="C30" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B31" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="C31" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="B32" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="C32" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="B33" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="C33" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="B34" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="C34" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="B35" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="C35" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="B36" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="C36" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="B37" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="C37" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B38" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="C38" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="B39" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="C39" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="B40" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="C40" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="B41" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="C41" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="B42" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="C42" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="B43" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="C43" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="B44" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="C44" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="B45" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="C45" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="B46" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="C46" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="B47" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="C47" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="B48" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="C48" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="B49" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="C49" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="B50" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="C50" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="B51" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="C51" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="B52" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="C52" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="B53" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="C53" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="B54" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="C54" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="C55" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="B56" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="B57" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="C57" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>245</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C58" t="s">
         <v>251</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="C58" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="B60" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="C60" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="B61" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="C61" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="B63" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="C63" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="C64" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="B66" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="C66" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="B67" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="C67" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="B68" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="C68" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="B69" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="C69" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="B70" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="C70" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="B71" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="C71" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="B72" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="C72" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="B73" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="C73" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="B74" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="C74" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="B75" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="C75" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="B76" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="C76" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="B77" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="C77" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="B78" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="C78" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="B79" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="C79" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="B80" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C80" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="B81" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="C81" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="B82" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="C82" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="B83" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="C83" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="B84" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="C84" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="B85" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="C85" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="B86" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="C86" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="B87" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="C87" t="s">
-        <v>398</v>
+        <v>392</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="B88" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="C88" t="s">
-        <v>399</v>
+        <v>393</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="B89" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="C89" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="B90" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="C90" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="B91" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="C91" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="B92" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="C92" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="B93" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="C93" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="B94" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="C94" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="B95" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="C95" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
       <c r="B102" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
       <c r="C102" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>407</v>
+        <v>401</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>408</v>
+        <v>402</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>520</v>
+        <v>512</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>415</v>
+        <v>409</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>416</v>
+        <v>410</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>418</v>
+        <v>412</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>419</v>
+        <v>413</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>521</v>
+        <v>513</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>519</v>
+        <v>511</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>420</v>
+        <v>414</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>522</v>
+        <v>514</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>518</v>
+        <v>510</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>421</v>
+        <v>415</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>523</v>
+        <v>515</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>524</v>
+        <v>516</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>525</v>
+        <v>517</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>429</v>
+        <v>423</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>428</v>
+        <v>422</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>427</v>
+        <v>421</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>430</v>
+        <v>424</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>422</v>
+        <v>416</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>431</v>
+        <v>425</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>425</v>
+        <v>419</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>433</v>
+        <v>427</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>436</v>
+        <v>430</v>
       </c>
       <c r="C115" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>432</v>
+        <v>426</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>437</v>
+        <v>431</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>426</v>
+        <v>420</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>434</v>
+        <v>428</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>439</v>
+        <v>433</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>438</v>
+        <v>432</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>440</v>
+        <v>434</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>441</v>
+        <v>435</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>442</v>
+        <v>436</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>443</v>
+        <v>437</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>444</v>
+        <v>438</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>445</v>
+        <v>439</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>447</v>
+        <v>441</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>451</v>
+        <v>445</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>452</v>
+        <v>446</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>453</v>
+        <v>447</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>454</v>
+        <v>448</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>455</v>
+        <v>449</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>456</v>
+        <v>450</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>457</v>
+        <v>451</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>468</v>
+        <v>462</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>470</v>
+        <v>464</v>
       </c>
       <c r="B125" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="C125" s="3" t="s">
         <v>459</v>
-      </c>
-      <c r="C125" s="3" t="s">
-        <v>465</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>471</v>
+        <v>465</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>464</v>
+        <v>458</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>469</v>
+        <v>463</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C127" s="3" t="s">
-        <v>466</v>
+        <v>460</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>472</v>
+        <v>466</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>467</v>
+        <v>461</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>475</v>
+        <v>469</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>473</v>
+        <v>467</v>
       </c>
       <c r="C129" s="3" t="s">
-        <v>474</v>
+        <v>468</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>476</v>
+        <v>470</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>480</v>
+        <v>474</v>
       </c>
       <c r="C130" s="3" t="s">
-        <v>484</v>
+        <v>478</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>477</v>
+        <v>471</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>481</v>
+        <v>475</v>
       </c>
       <c r="C131" s="3" t="s">
-        <v>485</v>
+        <v>676</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>478</v>
+        <v>472</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>483</v>
+        <v>477</v>
       </c>
       <c r="C132" t="s">
-        <v>486</v>
+        <v>479</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>479</v>
+        <v>473</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>482</v>
+        <v>476</v>
       </c>
       <c r="C133" t="s">
-        <v>487</v>
+        <v>675</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>488</v>
+        <v>480</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>490</v>
+        <v>482</v>
       </c>
       <c r="C134" s="3" t="s">
-        <v>489</v>
+        <v>481</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>491</v>
+        <v>483</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>492</v>
+        <v>484</v>
       </c>
       <c r="C135" s="3" t="s">
-        <v>493</v>
+        <v>485</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>494</v>
+        <v>486</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>495</v>
+        <v>487</v>
       </c>
       <c r="C136" s="3" t="s">
-        <v>496</v>
+        <v>488</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
       <c r="B137" t="s">
-        <v>498</v>
+        <v>490</v>
       </c>
       <c r="C137" s="3" t="s">
-        <v>499</v>
+        <v>491</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>502</v>
+        <v>494</v>
       </c>
       <c r="B138" t="s">
-        <v>500</v>
+        <v>492</v>
       </c>
       <c r="C138" s="3" t="s">
-        <v>501</v>
+        <v>493</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>503</v>
+        <v>495</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>504</v>
+        <v>496</v>
       </c>
       <c r="C139" t="s">
-        <v>505</v>
+        <v>497</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>506</v>
+        <v>498</v>
       </c>
       <c r="B140" t="s">
-        <v>507</v>
+        <v>499</v>
       </c>
       <c r="C140" s="3" t="s">
-        <v>508</v>
+        <v>500</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>509</v>
+        <v>501</v>
       </c>
       <c r="B141" t="s">
-        <v>510</v>
+        <v>502</v>
       </c>
       <c r="C141" s="3" t="s">
-        <v>511</v>
+        <v>503</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>570</v>
+        <v>562</v>
       </c>
       <c r="B142" t="s">
-        <v>571</v>
+        <v>563</v>
       </c>
       <c r="C142" s="3" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>572</v>
+        <v>564</v>
       </c>
       <c r="B143" t="s">
-        <v>576</v>
+        <v>568</v>
       </c>
       <c r="C143" s="3" t="s">
-        <v>585</v>
+        <v>577</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>573</v>
+        <v>565</v>
       </c>
       <c r="B144" t="s">
-        <v>577</v>
+        <v>569</v>
       </c>
       <c r="C144" s="3" t="s">
-        <v>586</v>
+        <v>578</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>574</v>
+        <v>566</v>
       </c>
       <c r="B145" t="s">
-        <v>578</v>
+        <v>570</v>
       </c>
       <c r="C145" s="3" t="s">
-        <v>587</v>
+        <v>579</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>575</v>
+        <v>567</v>
       </c>
       <c r="B146" t="s">
-        <v>579</v>
+        <v>571</v>
       </c>
       <c r="C146" s="3" t="s">
-        <v>588</v>
+        <v>580</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>582</v>
+        <v>574</v>
       </c>
       <c r="B147" t="s">
-        <v>581</v>
+        <v>573</v>
       </c>
       <c r="C147" t="s">
-        <v>584</v>
+        <v>576</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>580</v>
+        <v>572</v>
       </c>
       <c r="B148" t="s">
-        <v>583</v>
+        <v>575</v>
       </c>
       <c r="C148" t="s">
-        <v>589</v>
+        <v>581</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>596</v>
+        <v>588</v>
       </c>
       <c r="B149" t="s">
-        <v>597</v>
+        <v>589</v>
       </c>
       <c r="C149" s="3" t="s">
-        <v>598</v>
+        <v>590</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>621</v>
+        <v>613</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>622</v>
+        <v>614</v>
       </c>
       <c r="C150" s="3" t="s">
-        <v>592</v>
+        <v>584</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>623</v>
+        <v>615</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>594</v>
+        <v>586</v>
       </c>
       <c r="C151" s="3" t="s">
-        <v>595</v>
+        <v>587</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>624</v>
+        <v>616</v>
       </c>
       <c r="B152" t="s">
         <v>1</v>
       </c>
       <c r="C152" s="3" t="s">
-        <v>625</v>
+        <v>617</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>626</v>
+        <v>618</v>
       </c>
       <c r="B153" t="s">
         <v>2</v>
       </c>
       <c r="C153" s="3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>627</v>
+        <v>619</v>
       </c>
       <c r="B154" t="s">
-        <v>630</v>
+        <v>622</v>
       </c>
       <c r="C154" s="3" t="s">
-        <v>663</v>
+        <v>655</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>637</v>
+        <v>629</v>
       </c>
       <c r="B155" t="s">
-        <v>638</v>
+        <v>630</v>
       </c>
       <c r="C155" s="3" t="s">
-        <v>659</v>
+        <v>651</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>628</v>
+        <v>620</v>
       </c>
       <c r="B156" t="s">
-        <v>631</v>
+        <v>623</v>
       </c>
       <c r="C156" s="3" t="s">
-        <v>665</v>
+        <v>657</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>629</v>
+        <v>621</v>
       </c>
       <c r="B157" t="s">
-        <v>632</v>
+        <v>624</v>
       </c>
       <c r="C157" s="3" t="s">
-        <v>666</v>
+        <v>658</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>633</v>
+        <v>625</v>
       </c>
       <c r="B158" t="s">
-        <v>639</v>
+        <v>631</v>
       </c>
       <c r="C158" s="3" t="s">
-        <v>661</v>
+        <v>653</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>636</v>
+        <v>628</v>
       </c>
       <c r="B159" t="s">
-        <v>640</v>
+        <v>632</v>
       </c>
       <c r="C159" t="s">
-        <v>660</v>
+        <v>652</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>634</v>
+        <v>626</v>
       </c>
       <c r="B160" t="s">
-        <v>641</v>
+        <v>633</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>635</v>
+        <v>627</v>
       </c>
       <c r="B161" t="s">
-        <v>642</v>
+        <v>634</v>
       </c>
       <c r="C161" s="3" t="s">
-        <v>667</v>
+        <v>659</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>643</v>
+        <v>635</v>
       </c>
       <c r="B162" t="s">
-        <v>648</v>
+        <v>640</v>
       </c>
       <c r="C162" t="s">
-        <v>664</v>
+        <v>656</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>644</v>
+        <v>636</v>
       </c>
       <c r="B163" t="s">
-        <v>650</v>
+        <v>642</v>
       </c>
       <c r="C163" t="s">
-        <v>662</v>
+        <v>654</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>645</v>
+        <v>637</v>
       </c>
       <c r="B164" t="s">
-        <v>649</v>
+        <v>641</v>
       </c>
       <c r="C164" t="s">
-        <v>669</v>
+        <v>661</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>646</v>
+        <v>638</v>
       </c>
       <c r="B165" t="s">
-        <v>647</v>
+        <v>639</v>
       </c>
       <c r="C165" t="s">
-        <v>668</v>
+        <v>660</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>670</v>
+        <v>662</v>
       </c>
       <c r="B166" t="s">
         <v>22</v>

</xml_diff>